<commit_message>
Actualización 11 de febrero de 2024 - Lap HP
Se actualiza el repositorio con varios materiales.
</commit_message>
<xml_diff>
--- a/Bitacoras/NRC_124_Grupo_43/Parcial_03/Bitacora_Laboratorio_Parcial_03_NRC_125.xlsx
+++ b/Bitacoras/NRC_124_Grupo_43/Parcial_03/Bitacora_Laboratorio_Parcial_03_NRC_125.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusto\OneDrive\Documentos\Cursos_UVM\Plan PU\Fisica_3\Bitacoras\NRC_124_Grupo_43\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusto\OneDrive\Documentos\Cursos_UVM\Plan PU\Fisica_3\Bitacoras\NRC_124_Grupo_43\Parcial_03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB2B92C-C77F-4261-84DC-4FF2D5FEE6EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BFCE75F-C258-4FAE-96B2-A5F1679BCA05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{E9D7DD6B-2613-49CF-A776-8D7ABD912F27}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="70">
   <si>
     <t>Alumno</t>
   </si>
@@ -220,6 +220,33 @@
   </si>
   <si>
     <t>P5_Montaje</t>
+  </si>
+  <si>
+    <t>P6_Encuadre</t>
+  </si>
+  <si>
+    <t>P6_Montaje</t>
+  </si>
+  <si>
+    <t>P5_Reporte</t>
+  </si>
+  <si>
+    <t>P6_Reporte</t>
+  </si>
+  <si>
+    <t>Puntaje</t>
+  </si>
+  <si>
+    <t>Calificación</t>
+  </si>
+  <si>
+    <t>P5_Marco_Teórico</t>
+  </si>
+  <si>
+    <t>P7_Encuadre</t>
+  </si>
+  <si>
+    <t>P7_Montaje</t>
   </si>
 </sst>
 </file>
@@ -600,13 +627,13 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="11.42578125" style="2"/>
+    <col min="5" max="8" width="6.85546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -651,6 +678,9 @@
       <c r="E2" s="2">
         <v>1</v>
       </c>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -696,6 +726,9 @@
       <c r="D5" t="s">
         <v>19</v>
       </c>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -772,6 +805,9 @@
       <c r="E10" s="2">
         <v>1</v>
       </c>
+      <c r="G10" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -827,6 +863,9 @@
       </c>
       <c r="D14" t="s">
         <v>53</v>
+      </c>
+      <c r="G14" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -850,10 +889,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBAD8BD3-E3E4-4EEF-8F10-16C67BA87F20}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,10 +900,19 @@
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="11.42578125" style="2"/>
+    <col min="7" max="7" width="17.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" style="2"/>
+    <col min="13" max="13" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="2"/>
+    <col min="16" max="16" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -884,10 +932,37 @@
         <v>59</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -900,11 +975,33 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2">
+        <v>5</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2">
+        <v>5</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0</v>
+      </c>
+      <c r="O2" s="2">
+        <f>SUM(E2:M2)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -917,11 +1014,33 @@
       <c r="D3" t="s">
         <v>11</v>
       </c>
+      <c r="E3" s="2">
+        <v>4</v>
+      </c>
       <c r="F3" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="H3" s="2">
+        <v>5</v>
+      </c>
+      <c r="I3" s="2">
+        <v>4</v>
+      </c>
+      <c r="J3" s="2">
+        <v>5</v>
+      </c>
+      <c r="K3" s="2">
+        <v>5</v>
+      </c>
+      <c r="O3" s="2">
+        <f>SUM(E3:M3)</f>
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -934,11 +1053,33 @@
       <c r="D4" t="s">
         <v>15</v>
       </c>
+      <c r="E4" s="2">
+        <v>2.4</v>
+      </c>
       <c r="F4" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4" s="2">
+        <v>3.2</v>
+      </c>
+      <c r="H4" s="2">
+        <v>5</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <v>5</v>
+      </c>
+      <c r="K4" s="2">
+        <v>5</v>
+      </c>
+      <c r="O4" s="2">
+        <f>SUM(E4:M4)</f>
+        <v>20.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -951,11 +1092,33 @@
       <c r="D5" t="s">
         <v>19</v>
       </c>
+      <c r="E5" s="2">
+        <v>2.5</v>
+      </c>
       <c r="F5" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G5" s="2">
+        <v>4</v>
+      </c>
+      <c r="H5" s="2">
+        <v>5</v>
+      </c>
+      <c r="I5" s="2">
+        <v>3</v>
+      </c>
+      <c r="J5" s="2">
+        <v>5</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2">
+        <f>SUM(E5:M5)</f>
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -968,11 +1131,33 @@
       <c r="D6" t="s">
         <v>23</v>
       </c>
+      <c r="E6" s="2">
+        <v>4</v>
+      </c>
       <c r="F6" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G6" s="2">
+        <v>5</v>
+      </c>
+      <c r="H6" s="2">
+        <v>5</v>
+      </c>
+      <c r="I6" s="2">
+        <v>5</v>
+      </c>
+      <c r="J6" s="2">
+        <v>5</v>
+      </c>
+      <c r="K6" s="2">
+        <v>5</v>
+      </c>
+      <c r="O6" s="2">
+        <f>SUM(E6:M6)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -985,11 +1170,33 @@
       <c r="D7" t="s">
         <v>27</v>
       </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
       <c r="F7" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>5</v>
+      </c>
+      <c r="I7" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="J7" s="2">
+        <v>5</v>
+      </c>
+      <c r="K7" s="2">
+        <v>5</v>
+      </c>
+      <c r="O7" s="2">
+        <f>SUM(E7:M7)</f>
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1002,11 +1209,33 @@
       <c r="D8" t="s">
         <v>31</v>
       </c>
+      <c r="E8" s="2">
+        <v>4</v>
+      </c>
       <c r="F8" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8" s="2">
+        <v>5</v>
+      </c>
+      <c r="H8" s="2">
+        <v>5</v>
+      </c>
+      <c r="I8" s="2">
+        <v>5</v>
+      </c>
+      <c r="J8" s="2">
+        <v>5</v>
+      </c>
+      <c r="K8" s="2">
+        <v>5</v>
+      </c>
+      <c r="O8" s="2">
+        <f>SUM(E8:M8)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1019,11 +1248,33 @@
       <c r="D9" t="s">
         <v>35</v>
       </c>
+      <c r="E9" s="2">
+        <v>5</v>
+      </c>
       <c r="F9" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G9" s="2">
+        <v>5</v>
+      </c>
+      <c r="H9" s="2">
+        <v>5</v>
+      </c>
+      <c r="I9" s="2">
+        <v>5</v>
+      </c>
+      <c r="J9" s="2">
+        <v>5</v>
+      </c>
+      <c r="K9" s="2">
+        <v>5</v>
+      </c>
+      <c r="O9" s="2">
+        <f>SUM(E9:M9)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1036,11 +1287,33 @@
       <c r="D10" t="s">
         <v>39</v>
       </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
       <c r="F10" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2">
+        <v>5</v>
+      </c>
+      <c r="I10" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="J10" s="2">
+        <v>5</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0</v>
+      </c>
+      <c r="O10" s="2">
+        <f>SUM(E10:M10)</f>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -1053,11 +1326,33 @@
       <c r="D11" t="s">
         <v>42</v>
       </c>
+      <c r="E11" s="2">
+        <v>2.5</v>
+      </c>
       <c r="F11" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G11" s="2">
+        <v>5</v>
+      </c>
+      <c r="H11" s="2">
+        <v>5</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2">
+        <v>5</v>
+      </c>
+      <c r="K11" s="2">
+        <v>5</v>
+      </c>
+      <c r="O11" s="2">
+        <f>SUM(E11:M11)</f>
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -1070,11 +1365,33 @@
       <c r="D12" t="s">
         <v>45</v>
       </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
       <c r="F12" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G12" s="2">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2">
+        <v>5</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0</v>
+      </c>
+      <c r="J12" s="2">
+        <v>5</v>
+      </c>
+      <c r="K12" s="2">
+        <v>5</v>
+      </c>
+      <c r="O12" s="2">
+        <f>SUM(E12:M12)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -1087,11 +1404,33 @@
       <c r="D13" t="s">
         <v>49</v>
       </c>
+      <c r="E13" s="2">
+        <v>4</v>
+      </c>
       <c r="F13" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G13" s="2">
+        <v>5</v>
+      </c>
+      <c r="H13" s="2">
+        <v>5</v>
+      </c>
+      <c r="I13" s="2">
+        <v>5</v>
+      </c>
+      <c r="J13" s="2">
+        <v>5</v>
+      </c>
+      <c r="K13" s="2">
+        <v>5</v>
+      </c>
+      <c r="O13" s="2">
+        <f>SUM(E13:M13)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -1104,11 +1443,33 @@
       <c r="D14" t="s">
         <v>53</v>
       </c>
+      <c r="E14" s="2">
+        <v>4</v>
+      </c>
       <c r="F14" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G14" s="2">
+        <v>5</v>
+      </c>
+      <c r="H14" s="2">
+        <v>5</v>
+      </c>
+      <c r="I14" s="2">
+        <v>5</v>
+      </c>
+      <c r="J14" s="2">
+        <v>5</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0</v>
+      </c>
+      <c r="O14" s="2">
+        <f>SUM(E14:M14)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -1121,8 +1482,30 @@
       <c r="D15" t="s">
         <v>57</v>
       </c>
+      <c r="E15" s="2">
+        <v>5</v>
+      </c>
       <c r="F15" s="2">
         <v>5</v>
+      </c>
+      <c r="G15" s="2">
+        <v>5</v>
+      </c>
+      <c r="H15" s="2">
+        <v>5</v>
+      </c>
+      <c r="I15" s="2">
+        <v>5</v>
+      </c>
+      <c r="J15" s="2">
+        <v>5</v>
+      </c>
+      <c r="K15" s="2">
+        <v>5</v>
+      </c>
+      <c r="O15" s="2">
+        <f>SUM(E15:M15)</f>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>